<commit_message>
Updated plotting code to separate customer charges by utility
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -332,11 +332,17 @@
   <si>
     <t>Industrial Rate B-20 at Primary Voltage</t>
   </si>
+  <si>
+    <t>PDP cha</t>
+  </si>
+  <si>
+    <t>PDP charges ignored</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" count="8" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
@@ -732,7 +738,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView topLeftCell="A36" workbookViewId="0" tabSelected="1">
-      <selection pane="topLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -828,7 +834,7 @@
         <v>36001010006</v>
       </c>
     </row>
-    <row ht="30" r="6" spans="1:15">
+    <row r="6">
       <c r="A6" s="3" t="s">
         <v>100</v>
       </c>
@@ -851,121 +857,121 @@
         <v>6002121001</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row ht="30" r="7" spans="1:15">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="B7" s="2">
-        <v>34006012001</v>
+        <v>6005025001</v>
       </c>
       <c r="C7" s="2">
-        <v>34001005001</v>
+        <v>6005053001</v>
       </c>
       <c r="D7" s="2">
-        <v>34001030001</v>
+        <v>6002032003</v>
       </c>
       <c r="E7" s="2">
-        <v>34001082001</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+        <v>6002036001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6002041001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>6002121001</v>
+      </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2">
+        <v>34006012001</v>
+      </c>
+      <c r="C8" s="2">
+        <v>34001005001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>34001030001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>34001082001</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
         <v>6004010004</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>6004009003</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>6008022001</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="2">
         <v>6008022002</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <v>6004010001</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <v>6004009001</v>
       </c>
     </row>
-    <row ht="30" r="9" spans="1:15">
-      <c r="A9" s="3" t="s">
+    <row ht="30" r="10" spans="1:15">
+      <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>36002001007</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
         <v>36002001004</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="2">
         <v>36002001006</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E10" s="2">
         <v>36003169012</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F10" s="2">
         <v>36002001010</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G10" s="2">
         <v>36002001009</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H10" s="2">
         <v>36002001005</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I10" s="2">
         <v>36002001002</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J10" s="2">
         <v>36002001003</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K10" s="2">
         <v>36002001012</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L10" s="2">
         <v>36002001001</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M10" s="2">
         <v>36002001011</v>
       </c>
     </row>
-    <row ht="15" customHeight="1" r="10" spans="1:15">
-      <c r="A10" s="3" t="s">
+    <row ht="15" customHeight="1" r="11" spans="1:15">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
         <v>53001280001</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row ht="15" customHeight="1" r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2">
-        <v>42000094003</v>
-      </c>
-      <c r="C11" s="2">
-        <v>42000094001</v>
-      </c>
-      <c r="D11" s="2">
-        <v>42000094002</v>
-      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -976,15 +982,19 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row ht="30" customHeight="1" r="12" spans="1:15">
-      <c r="A12" s="3" t="s">
-        <v>25</v>
+    <row ht="15" customHeight="1" r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>24</v>
       </c>
       <c r="B12" s="2">
-        <v>53000776002</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+        <v>42000094003</v>
+      </c>
+      <c r="C12" s="2">
+        <v>42000094001</v>
+      </c>
+      <c r="D12" s="2">
+        <v>42000094002</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -995,12 +1005,12 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row ht="15" customHeight="1" r="13" spans="1:15">
+    <row ht="30" customHeight="1" r="13" spans="1:15">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2">
-        <v>39001666001</v>
+        <v>53000776002</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1014,25 +1024,17 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row ht="30" customHeight="1" r="14" spans="1:15">
+    <row ht="15" customHeight="1" r="14" spans="1:15">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2">
-        <v>39001666002</v>
-      </c>
-      <c r="C14" s="2">
-        <v>39000084001</v>
-      </c>
-      <c r="D14" s="2">
-        <v>39008260001</v>
-      </c>
-      <c r="E14" s="2">
-        <v>10000027001</v>
-      </c>
-      <c r="F14" s="2">
-        <v>34002065001</v>
-      </c>
+        <v>39001666001</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1041,23 +1043,25 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row ht="15" customHeight="1" r="15" spans="1:15">
+    <row ht="30" customHeight="1" r="15" spans="1:15">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2">
-        <v>12000001001</v>
+        <v>39001666002</v>
       </c>
       <c r="C15" s="2">
-        <v>12000017028</v>
+        <v>39000084001</v>
       </c>
       <c r="D15" s="2">
-        <v>12000017027</v>
+        <v>39008260001</v>
       </c>
       <c r="E15" s="2">
-        <v>12000017004</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>10000027001</v>
+      </c>
+      <c r="F15" s="2">
+        <v>34002065001</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1068,16 +1072,20 @@
     </row>
     <row ht="15" customHeight="1" r="16" spans="1:15">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
-        <v>47000940001</v>
+        <v>12000001001</v>
       </c>
       <c r="C16" s="2">
-        <v>47000940002</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+        <v>12000017028</v>
+      </c>
+      <c r="D16" s="2">
+        <v>12000017027</v>
+      </c>
+      <c r="E16" s="2">
+        <v>12000017004</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1087,14 +1095,16 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row ht="15" customHeight="1" r="17" spans="1:13">
+    <row ht="15" customHeight="1" r="17" spans="1:15">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2">
-        <v>47000245002</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>47000940001</v>
+      </c>
+      <c r="C17" s="2">
+        <v>47000940002</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1108,10 +1118,10 @@
     </row>
     <row ht="15" customHeight="1" r="18" spans="1:13">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2">
-        <v>40000123012</v>
+        <v>47000245002</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1127,10 +1137,10 @@
     </row>
     <row ht="15" customHeight="1" r="19" spans="1:13">
       <c r="A19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2">
-        <v>32000011001</v>
+        <v>40000123012</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1146,10 +1156,10 @@
     </row>
     <row ht="15" customHeight="1" r="20" spans="1:13">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2">
-        <v>41000017001</v>
+        <v>32000011001</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1163,16 +1173,14 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row ht="30" customHeight="1" r="21" spans="1:13">
+    <row ht="15" customHeight="1" r="21" spans="1:13">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2">
-        <v>26000596001</v>
-      </c>
-      <c r="C21" s="2">
-        <v>26004005011</v>
-      </c>
+        <v>41000017001</v>
+      </c>
+      <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1184,19 +1192,17 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row ht="15" customHeight="1" r="22" spans="1:13">
+    <row ht="30" customHeight="1" r="22" spans="1:13">
       <c r="A22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2">
-        <v>29001023001</v>
+        <v>26000596001</v>
       </c>
       <c r="C22" s="2">
-        <v>29001023002</v>
-      </c>
-      <c r="D22" s="2">
-        <v>27000001001</v>
-      </c>
+        <v>26004005011</v>
+      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1209,20 +1215,18 @@
     </row>
     <row ht="15" customHeight="1" r="23" spans="1:13">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="2">
-        <v>48004026002</v>
+        <v>29001023001</v>
       </c>
       <c r="C23" s="2">
-        <v>48004026001</v>
+        <v>29001023002</v>
       </c>
       <c r="D23" s="2">
-        <v>48000004001</v>
-      </c>
-      <c r="E23" s="2">
-        <v>48004122001</v>
-      </c>
+        <v>27000001001</v>
+      </c>
+      <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1234,14 +1238,20 @@
     </row>
     <row ht="15" customHeight="1" r="24" spans="1:13">
       <c r="A24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2">
-        <v>8000070001</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+        <v>48004026002</v>
+      </c>
+      <c r="C24" s="2">
+        <v>48004026001</v>
+      </c>
+      <c r="D24" s="2">
+        <v>48000004001</v>
+      </c>
+      <c r="E24" s="2">
+        <v>48004122001</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1253,10 +1263,10 @@
     </row>
     <row ht="15" customHeight="1" r="25" spans="1:13">
       <c r="A25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2">
-        <v>42006056001</v>
+        <v>8000070001</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1270,12 +1280,12 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row ht="30" customHeight="1" r="26" spans="1:13">
+    <row ht="15" customHeight="1" r="26" spans="1:13">
       <c r="A26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2">
-        <v>53000776001</v>
+        <v>42006056001</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1291,10 +1301,10 @@
     </row>
     <row ht="30" customHeight="1" r="27" spans="1:13">
       <c r="A27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2">
-        <v>11000001001</v>
+        <v>53000776001</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1308,12 +1318,12 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row ht="15" customHeight="1" r="28" spans="1:13">
+    <row ht="30" customHeight="1" r="28" spans="1:13">
       <c r="A28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2">
-        <v>25000128001</v>
+        <v>11000001001</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1327,16 +1337,14 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row ht="30" customHeight="1" r="29" spans="1:13">
+    <row ht="15" customHeight="1" r="29" spans="1:13">
       <c r="A29" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2">
-        <v>39001792001</v>
-      </c>
-      <c r="C29" s="2">
-        <v>39001792002</v>
-      </c>
+        <v>25000128001</v>
+      </c>
+      <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1350,12 +1358,14 @@
     </row>
     <row ht="30" customHeight="1" r="30" spans="1:13">
       <c r="A30" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="2">
-        <v>29001011001</v>
-      </c>
-      <c r="C30" s="2"/>
+        <v>39001792001</v>
+      </c>
+      <c r="C30" s="2">
+        <v>39001792002</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1369,10 +1379,10 @@
     </row>
     <row ht="30" customHeight="1" r="31" spans="1:13">
       <c r="A31" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="2">
-        <v>55003100001</v>
+        <v>29001011001</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1386,12 +1396,12 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row ht="15" customHeight="1" r="32" spans="1:13">
+    <row ht="30" customHeight="1" r="32" spans="1:13">
       <c r="A32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="2">
-        <v>21000025001</v>
+        <v>55003100001</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1405,12 +1415,12 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row ht="15" customHeight="1" r="33" spans="1:15">
+    <row ht="15" customHeight="1" r="33" spans="1:13">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="2">
-        <v>42005016001</v>
+        <v>21000025001</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1426,10 +1436,10 @@
     </row>
     <row ht="15" customHeight="1" r="34" spans="1:15">
       <c r="A34" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="2">
-        <v>6005009001</v>
+        <v>42005016001</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1443,12 +1453,12 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:15">
+    <row ht="15" customHeight="1" r="35" spans="1:15">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="2">
-        <v>6009031001</v>
+        <v>6005009001</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1462,256 +1472,275 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row ht="30" r="36" spans="1:15">
+    <row r="36" spans="1:15">
       <c r="A36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="2">
+        <v>6009031001</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row ht="30" r="37" spans="1:15">
+      <c r="A37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B37" s="2">
         <v>31001825002</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
-      <c r="A37" t="s">
+    <row r="38" spans="1:15">
+      <c r="A38" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B38" s="2">
         <v>36007136001</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C38" s="2">
         <v>36008024001</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D38" s="2">
         <v>36009071001</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E38" s="2">
         <v>17000721009</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F38" s="2">
         <v>17000721007</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G38" s="2">
         <v>17000721001</v>
       </c>
     </row>
-    <row ht="30" customHeight="1" r="38" spans="1:15">
-      <c r="A38" s="3" t="s">
+    <row ht="30" customHeight="1" r="39" spans="1:15">
+      <c r="A39" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B38" s="2">
-        <v>9000641001</v>
-      </c>
-      <c r="C38" s="2">
-        <v>42006056001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="A39" t="s">
-        <v>52</v>
       </c>
       <c r="B39" s="2">
         <v>9000641001</v>
       </c>
       <c r="C39" s="2">
+        <v>42006056001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="2">
+        <v>9000641001</v>
+      </c>
+      <c r="C40" s="2">
         <v>51000161001</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D40" s="2">
         <v>51000154002</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E40" s="2">
         <v>39001666001</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F40" s="2">
         <v>39001666002</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G40" s="2">
         <v>39000084001</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H40" s="2">
         <v>39008260001</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I40" s="2">
         <v>39001792001</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J40" s="2">
         <v>39001792002</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K40" s="2">
         <v>29001023001</v>
       </c>
-      <c r="L39" s="2">
+      <c r="L40" s="2">
         <v>29001023002</v>
       </c>
-      <c r="M39" s="2">
+      <c r="M40" s="2">
         <v>53000776001</v>
       </c>
-      <c r="N39" s="2">
+      <c r="N40" s="2">
         <v>47001016001</v>
       </c>
-      <c r="O39" s="2">
+      <c r="O40" s="2">
         <v>6009031001</v>
-      </c>
-    </row>
-    <row ht="30" r="40" spans="1:15">
-      <c r="A40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" s="2">
-        <v>48003033002</v>
-      </c>
-      <c r="C40" s="2">
-        <v>9000641001</v>
-      </c>
-      <c r="D40" s="2">
-        <v>12000001001</v>
-      </c>
-      <c r="E40" s="2">
-        <v>12000017028</v>
-      </c>
-      <c r="F40" s="2">
-        <v>12000017027</v>
-      </c>
-      <c r="G40" s="2">
-        <v>12000017004</v>
-      </c>
-      <c r="H40" s="2">
-        <v>32000011001</v>
-      </c>
-      <c r="I40" s="2">
-        <v>32000200820</v>
-      </c>
-      <c r="J40" s="2">
-        <v>41000017001</v>
-      </c>
-      <c r="K40" s="2">
-        <v>24000001002</v>
-      </c>
-      <c r="L40" s="2">
-        <v>26000596001</v>
-      </c>
-      <c r="M40" s="2">
-        <v>26004005011</v>
       </c>
     </row>
     <row ht="30" r="41" spans="1:15">
       <c r="A41" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" s="2">
         <v>48003033002</v>
       </c>
       <c r="C41" s="2">
+        <v>9000641001</v>
+      </c>
+      <c r="D41" s="2">
         <v>12000001001</v>
       </c>
-      <c r="D41" s="2">
+      <c r="E41" s="2">
         <v>12000017028</v>
       </c>
-      <c r="E41" s="2">
+      <c r="F41" s="2">
         <v>12000017027</v>
       </c>
-      <c r="F41" s="2">
+      <c r="G41" s="2">
         <v>12000017004</v>
       </c>
-      <c r="G41" s="2">
+      <c r="H41" s="2">
+        <v>32000011001</v>
+      </c>
+      <c r="I41" s="2">
+        <v>32000200820</v>
+      </c>
+      <c r="J41" s="2">
         <v>41000017001</v>
       </c>
-      <c r="H41" s="2">
-        <v>34002065001</v>
+      <c r="K41" s="2">
+        <v>24000001002</v>
+      </c>
+      <c r="L41" s="2">
+        <v>26000596001</v>
+      </c>
+      <c r="M41" s="2">
+        <v>26004005011</v>
       </c>
     </row>
     <row ht="30" r="42" spans="1:15">
       <c r="A42" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42" s="2">
-        <v>47000940001</v>
+        <v>48003033002</v>
       </c>
       <c r="C42" s="2">
-        <v>47000940002</v>
+        <v>12000001001</v>
       </c>
       <c r="D42" s="2">
-        <v>47000245002</v>
+        <v>12000017028</v>
       </c>
       <c r="E42" s="2">
-        <v>26000596001</v>
+        <v>12000017027</v>
       </c>
       <c r="F42" s="2">
-        <v>26004005011</v>
+        <v>12000017004</v>
       </c>
       <c r="G42" s="2">
-        <v>29001011001</v>
+        <v>41000017001</v>
       </c>
       <c r="H42" s="2">
-        <v>47001016001</v>
+        <v>34002065001</v>
       </c>
     </row>
     <row ht="30" r="43" spans="1:15">
       <c r="A43" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" s="2">
-        <v>29001023001</v>
+        <v>47000940001</v>
       </c>
       <c r="C43" s="2">
-        <v>29001023002</v>
+        <v>47000940002</v>
       </c>
       <c r="D43" s="2">
-        <v>42006056001</v>
+        <v>47000245002</v>
+      </c>
+      <c r="E43" s="2">
+        <v>26000596001</v>
+      </c>
+      <c r="F43" s="2">
+        <v>26004005011</v>
+      </c>
+      <c r="G43" s="2">
+        <v>29001011001</v>
+      </c>
+      <c r="H43" s="2">
+        <v>47001016001</v>
       </c>
     </row>
     <row ht="30" r="44" spans="1:15">
       <c r="A44" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="2">
-        <v>26000596001</v>
+        <v>29001023001</v>
       </c>
       <c r="C44" s="2">
-        <v>26004005011</v>
+        <v>29001023002</v>
+      </c>
+      <c r="D44" s="2">
+        <v>42006056001</v>
       </c>
     </row>
     <row ht="30" r="45" spans="1:15">
       <c r="A45" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" s="2">
-        <v>39002093001</v>
+        <v>26000596001</v>
+      </c>
+      <c r="C45" s="2">
+        <v>26004005011</v>
       </c>
     </row>
     <row ht="30" r="46" spans="1:15">
       <c r="A46" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46" s="2">
-        <v>10000027001</v>
+        <v>39002093001</v>
       </c>
     </row>
     <row ht="30" r="47" spans="1:15">
       <c r="A47" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47" s="2">
         <v>10000027001</v>
       </c>
-      <c r="C47" s="2">
-        <v>13000012004</v>
-      </c>
     </row>
     <row ht="30" r="48" spans="1:15">
       <c r="A48" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48" s="2">
         <v>10000027001</v>
       </c>
       <c r="C48" s="2">
+        <v>13000012004</v>
+      </c>
+    </row>
+    <row ht="30" r="49" spans="1:15">
+      <c r="A49" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="2">
+        <v>10000027001</v>
+      </c>
+      <c r="C49" s="2">
         <v>29001011001</v>
       </c>
     </row>
-    <row ht="45" r="49" spans="1:2">
-      <c r="A49" s="3" t="s">
+    <row ht="45" r="50" spans="1:2">
+      <c r="A50" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B50" s="2">
         <v>6009031001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed typo of CWS to CWNS
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fletc\Git\wwtp-energy-rates\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-rates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8389C2-D65E-4C1A-A427-AB2C91D1AE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F7CBF6-E727-0244-A9F0-C2DF867D6EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electric" sheetId="1" r:id="rId1"/>
@@ -33,53 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="102">
   <si>
     <t>Assumption</t>
   </si>
   <si>
-    <t>CWS_No_1</t>
-  </si>
-  <si>
-    <t>CWS_No_2</t>
-  </si>
-  <si>
-    <t>CWS_No_3</t>
-  </si>
-  <si>
-    <t>CWS_No_4</t>
-  </si>
-  <si>
-    <t>CWS_No_5</t>
-  </si>
-  <si>
-    <t>CWS_No_6</t>
-  </si>
-  <si>
-    <t>CWS_No_7</t>
-  </si>
-  <si>
-    <t>CWS_No_8</t>
-  </si>
-  <si>
-    <t>CWS_No_9</t>
-  </si>
-  <si>
-    <t>CWS_No_10</t>
-  </si>
-  <si>
-    <t>CWS_No_11</t>
-  </si>
-  <si>
-    <t>CWS_No_12</t>
-  </si>
-  <si>
-    <t>CWS_No_13</t>
-  </si>
-  <si>
-    <t>CWS_No_14</t>
-  </si>
-  <si>
     <t>Rate Schedule GSDT</t>
   </si>
   <si>
@@ -339,6 +297,48 @@
   </si>
   <si>
     <t>Large rate category</t>
+  </si>
+  <si>
+    <t>CWNS_No_1</t>
+  </si>
+  <si>
+    <t>CWNS_No_2</t>
+  </si>
+  <si>
+    <t>CWNS_No_3</t>
+  </si>
+  <si>
+    <t>CWNS_No_4</t>
+  </si>
+  <si>
+    <t>CWNS_No_5</t>
+  </si>
+  <si>
+    <t>CWNS_No_6</t>
+  </si>
+  <si>
+    <t>CWNS_No_7</t>
+  </si>
+  <si>
+    <t>CWNS_No_8</t>
+  </si>
+  <si>
+    <t>CWNS_No_9</t>
+  </si>
+  <si>
+    <t>CWNS_No_10</t>
+  </si>
+  <si>
+    <t>CWNS_No_11</t>
+  </si>
+  <si>
+    <t>CWNS_No_12</t>
+  </si>
+  <si>
+    <t>CWNS_No_13</t>
+  </si>
+  <si>
+    <t>CWNS_No_14</t>
   </si>
 </sst>
 </file>
@@ -365,12 +365,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -727,92 +729,92 @@
   </sheetPr>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="2" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
       <c r="B2">
         <v>12000053001</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>48003033002</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>31001825002</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>36001010001</v>
@@ -824,9 +826,9 @@
         <v>36001010006</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B6" s="2">
         <v>6005025001</v>
@@ -847,9 +849,9 @@
         <v>6002121001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B7" s="2">
         <v>6005025001</v>
@@ -870,9 +872,9 @@
         <v>6002121001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>34006012001</v>
@@ -889,9 +891,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
         <v>6004010004</v>
@@ -912,9 +914,9 @@
         <v>6004009001</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2">
         <v>36002001007</v>
@@ -953,9 +955,9 @@
         <v>36002001011</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>53001280001</v>
@@ -972,9 +974,9 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B12" s="2">
         <v>32000200820</v>
@@ -993,9 +995,9 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2">
         <v>42000094003</v>
@@ -1016,9 +1018,9 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B14" s="2">
         <v>53000776002</v>
@@ -1035,9 +1037,9 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2">
         <v>39001666001</v>
@@ -1054,9 +1056,9 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2">
         <v>39001666002</v>
@@ -1081,9 +1083,9 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2">
         <v>12000001001</v>
@@ -1106,9 +1108,9 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2">
         <v>47000940001</v>
@@ -1127,9 +1129,9 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B19" s="2">
         <v>47000245002</v>
@@ -1146,9 +1148,9 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B20" s="2">
         <v>40000123012</v>
@@ -1165,9 +1167,9 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B21" s="2">
         <v>32000011001</v>
@@ -1184,9 +1186,9 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B22" s="2">
         <v>41000017001</v>
@@ -1203,9 +1205,9 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2">
         <v>26000596001</v>
@@ -1224,9 +1226,9 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B24" s="2">
         <v>29001023001</v>
@@ -1247,9 +1249,9 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B25" s="2">
         <v>48004026002</v>
@@ -1272,9 +1274,9 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2">
         <v>8000070001</v>
@@ -1291,9 +1293,9 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2">
         <v>42006056001</v>
@@ -1310,9 +1312,9 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2">
         <v>53000776001</v>
@@ -1329,9 +1331,9 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B29" s="2">
         <v>11000001001</v>
@@ -1348,9 +1350,9 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B30" s="2">
         <v>25000128001</v>
@@ -1367,9 +1369,9 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B31" s="2">
         <v>51000161001</v>
@@ -1388,9 +1390,9 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B32" s="2">
         <v>39001792001</v>
@@ -1409,9 +1411,9 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B33" s="2">
         <v>29001011001</v>
@@ -1428,9 +1430,9 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B34" s="2">
         <v>55003100001</v>
@@ -1447,9 +1449,9 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B35" s="2">
         <v>21000025001</v>
@@ -1466,9 +1468,9 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B36" s="2">
         <v>42005016001</v>
@@ -1485,9 +1487,9 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B37" s="2">
         <v>6005009001</v>
@@ -1504,9 +1506,9 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B38" s="2">
         <v>6009031001</v>
@@ -1523,17 +1525,17 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B39" s="2">
         <v>31001825002</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B40" s="2">
         <v>36007136001</v>
@@ -1554,9 +1556,9 @@
         <v>17000721001</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B41" s="2">
         <v>9000641001</v>
@@ -1565,9 +1567,9 @@
         <v>42006056001</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B42" s="2">
         <v>9000641001</v>
@@ -1612,9 +1614,9 @@
         <v>6009031001</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B43" s="2">
         <v>48003033002</v>
@@ -1653,9 +1655,9 @@
         <v>26004005011</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B44" s="2">
         <v>48003033002</v>
@@ -1679,9 +1681,9 @@
         <v>34002065001</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B45" s="2">
         <v>47000940001</v>
@@ -1705,9 +1707,9 @@
         <v>47001016001</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B46" s="2">
         <v>29001023001</v>
@@ -1719,9 +1721,9 @@
         <v>42006056001</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B47" s="2">
         <v>26000596001</v>
@@ -1730,25 +1732,25 @@
         <v>26004005011</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B48" s="2">
         <v>39002093001</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B49" s="2">
         <v>10000027001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B50" s="2">
         <v>10000027001</v>
@@ -1757,9 +1759,9 @@
         <v>13000012004</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B51" s="2">
         <v>10000027001</v>
@@ -1768,9 +1770,9 @@
         <v>29001011001</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B52" s="2">
         <v>6009031001</v>
@@ -1784,54 +1786,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85995C10-2ADA-4E06-99AB-80C6038BFB63}">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.140625" customWidth="1"/>
-    <col min="2" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.1640625" customWidth="1"/>
+    <col min="2" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2">
         <v>29001023001</v>
@@ -1840,9 +1839,9 @@
         <v>29001023002</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2">
         <v>36007136001</v>
@@ -1854,17 +1853,17 @@
         <v>36009071001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2">
         <v>8000070001</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2">
         <v>53001280001</v>
@@ -1876,9 +1875,9 @@
         <v>53000776002</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B6" s="2">
         <v>11000001001</v>
@@ -1889,9 +1888,9 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2">
         <v>25000128001</v>
@@ -1902,9 +1901,9 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2">
         <v>39002093001</v>
@@ -1915,9 +1914,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B9" s="2">
         <v>39001792001</v>
@@ -1932,9 +1931,9 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B10" s="2">
         <v>47001016001</v>
@@ -1945,9 +1944,9 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B11" s="2">
         <v>36002001007</v>
@@ -1970,12 +1969,12 @@
       <c r="H11" s="2">
         <v>36002001011</v>
       </c>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B12" s="2">
         <v>36002001006</v>
@@ -1992,10 +1991,10 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>34001005001</v>
       </c>
@@ -2005,12 +2004,12 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B14" s="2">
         <v>6002032003</v>
@@ -2029,12 +2028,12 @@
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B15" s="2">
         <v>36002001006</v>
@@ -2051,12 +2050,12 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B16" s="2">
         <v>11000001001</v>
@@ -2067,9 +2066,9 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2">
         <v>39002093001</v>
@@ -2086,9 +2085,9 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B18" s="2">
         <v>12000053001</v>
@@ -2099,9 +2098,9 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2">
         <v>12000001001</v>
@@ -2116,11 +2115,10 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2">
         <v>35000021001</v>
@@ -2135,11 +2133,10 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B21" s="2">
         <v>10000027001</v>
@@ -2154,11 +2151,10 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B22" s="2">
         <v>41000017001</v>
@@ -2173,11 +2169,10 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B23" s="2">
         <v>12000017027</v>
@@ -2194,11 +2189,10 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B24" s="2">
         <v>6008022001</v>
@@ -2219,11 +2213,10 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B25" s="2">
         <v>15000003001</v>
@@ -2238,11 +2231,10 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B26" s="2">
         <v>36003169012</v>
@@ -2257,11 +2249,10 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2">
         <v>48004026002</v>
@@ -2276,11 +2267,10 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-    </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B28" s="2">
         <v>39000084001</v>
@@ -2295,11 +2285,10 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B29" s="2">
         <v>55003100001</v>
@@ -2314,11 +2303,10 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-    </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B30" s="2">
         <v>42000094002</v>
@@ -2333,11 +2321,10 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-    </row>
-    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B31" s="2">
         <v>6009031001</v>
@@ -2352,11 +2339,10 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2">
         <v>13000012004</v>
@@ -2371,11 +2357,10 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-    </row>
-    <row r="33" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B33" s="2">
         <v>4001318001</v>
@@ -2390,11 +2375,10 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-    </row>
-    <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B34" s="2">
         <v>6005009001</v>
@@ -2417,14 +2401,13 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2436,14 +2419,13 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-    </row>
-    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2455,14 +2437,13 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2474,9 +2455,8 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-    </row>
-    <row r="38" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2489,9 +2469,8 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-    </row>
-    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2504,9 +2483,8 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-    </row>
-    <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2519,9 +2497,8 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-    </row>
-    <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2534,9 +2511,8 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-    </row>
-    <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2549,9 +2525,8 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-    </row>
-    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2564,9 +2539,8 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-    </row>
-    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2579,13 +2553,12 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2594,10 +2567,10 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2605,7 +2578,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2614,9 +2587,8 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2625,13 +2597,13 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added generation charges to SCE rates
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6751E4E5-BEB2-D740-A442-987CB19AF496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B4B1B9-0FDF-4C4C-9E55-778BE294A9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Rate: LPL-Primary</t>
   </si>
   <si>
-    <t>Rate TOU-8 at 2-50 kV</t>
-  </si>
-  <si>
     <t>Service Class 9: Rate II - General - Large - Time-of-Day</t>
   </si>
   <si>
@@ -342,6 +339,9 @@
   </si>
   <si>
     <t>Rider GEN - Time of Day Option</t>
+  </si>
+  <si>
+    <t>Rate TOU-8 at 2-50 kV - Option E</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -413,7 +413,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,8 +732,8 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -750,46 +749,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -832,7 +831,7 @@
     </row>
     <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="2">
         <v>6005025001</v>
@@ -855,7 +854,7 @@
     </row>
     <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2">
         <v>6005025001</v>
@@ -897,7 +896,7 @@
     </row>
     <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="B9" s="2">
         <v>6004010004</v>
@@ -920,7 +919,7 @@
     </row>
     <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>36002001007</v>
@@ -961,7 +960,7 @@
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
         <v>53001280001</v>
@@ -980,7 +979,7 @@
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="2">
         <v>32000200820</v>
@@ -1001,7 +1000,7 @@
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>42000094003</v>
@@ -1024,7 +1023,7 @@
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="2">
         <v>53000776002</v>
@@ -1043,7 +1042,7 @@
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2">
         <v>39001666001</v>
@@ -1062,7 +1061,7 @@
     </row>
     <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="2">
         <v>39001666002</v>
@@ -1089,7 +1088,7 @@
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="2">
         <v>12000001001</v>
@@ -1114,7 +1113,7 @@
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="2">
         <v>47000940001</v>
@@ -1135,7 +1134,7 @@
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2">
         <v>47000245002</v>
@@ -1154,7 +1153,7 @@
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="2">
         <v>40000123012</v>
@@ -1173,7 +1172,7 @@
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="2">
         <v>32000011001</v>
@@ -1192,7 +1191,7 @@
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="2">
         <v>41000017001</v>
@@ -1211,7 +1210,7 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="2">
         <v>26000596001</v>
@@ -1232,7 +1231,7 @@
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="2">
         <v>29001023001</v>
@@ -1255,7 +1254,7 @@
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="2">
         <v>48004026002</v>
@@ -1280,7 +1279,7 @@
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="2">
         <v>8000070001</v>
@@ -1299,7 +1298,7 @@
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="2">
         <v>42006056001</v>
@@ -1318,7 +1317,7 @@
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="2">
         <v>53000776001</v>
@@ -1337,7 +1336,7 @@
     </row>
     <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="2">
         <v>11000001001</v>
@@ -1356,7 +1355,7 @@
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="2">
         <v>25000128001</v>
@@ -1375,7 +1374,7 @@
     </row>
     <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" s="2">
         <v>51000161001</v>
@@ -1396,7 +1395,7 @@
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="2">
         <v>39001792001</v>
@@ -1417,7 +1416,7 @@
     </row>
     <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="2">
         <v>29001011001</v>
@@ -1436,7 +1435,7 @@
     </row>
     <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="2">
         <v>55003100001</v>
@@ -1455,7 +1454,7 @@
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="2">
         <v>21000025001</v>
@@ -1474,7 +1473,7 @@
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" s="2">
         <v>42005016001</v>
@@ -1493,7 +1492,7 @@
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" s="2">
         <v>6005009001</v>
@@ -1512,7 +1511,7 @@
     </row>
     <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B38" s="2">
         <v>6009031001</v>
@@ -1531,7 +1530,7 @@
     </row>
     <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="2">
         <v>31001825002</v>
@@ -1539,7 +1538,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" s="2">
         <v>36007136001</v>
@@ -1562,7 +1561,7 @@
     </row>
     <row r="41" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B41" s="2">
         <v>9000641001</v>
@@ -1573,7 +1572,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="2">
         <v>9000641001</v>
@@ -1620,7 +1619,7 @@
     </row>
     <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43" s="2">
         <v>48003033002</v>
@@ -1661,7 +1660,7 @@
     </row>
     <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="2">
         <v>48003033002</v>
@@ -1687,7 +1686,7 @@
     </row>
     <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="2">
         <v>47000940001</v>
@@ -1713,7 +1712,7 @@
     </row>
     <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="2">
         <v>29001023001</v>
@@ -1727,7 +1726,7 @@
     </row>
     <row r="47" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B47" s="2">
         <v>26000596001</v>
@@ -1738,7 +1737,7 @@
     </row>
     <row r="48" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="2">
         <v>39002093001</v>
@@ -1746,7 +1745,7 @@
     </row>
     <row r="49" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B49" s="2">
         <v>10000027001</v>
@@ -1754,7 +1753,7 @@
     </row>
     <row r="50" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" s="2">
         <v>10000027001</v>
@@ -1765,7 +1764,7 @@
     </row>
     <row r="51" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="2">
         <v>10000027001</v>
@@ -1776,7 +1775,7 @@
     </row>
     <row r="52" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" s="2">
         <v>6009031001</v>
@@ -1784,9 +1783,9 @@
     </row>
     <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" s="6">
+        <v>101</v>
+      </c>
+      <c r="B53">
         <v>39000084001</v>
       </c>
     </row>
@@ -1815,25 +1814,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1842,7 +1841,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2">
         <v>29001023001</v>
@@ -1853,7 +1852,7 @@
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2">
         <v>36007136001</v>
@@ -1867,7 +1866,7 @@
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2">
         <v>8000070001</v>
@@ -1875,7 +1874,7 @@
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2">
         <v>53001280001</v>
@@ -1889,7 +1888,7 @@
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2">
         <v>11000001001</v>
@@ -1902,7 +1901,7 @@
     </row>
     <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2">
         <v>25000128001</v>
@@ -1915,7 +1914,7 @@
     </row>
     <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="2">
         <v>39002093001</v>
@@ -1928,7 +1927,7 @@
     </row>
     <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2">
         <v>39001792001</v>
@@ -1945,7 +1944,7 @@
     </row>
     <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2">
         <v>47001016001</v>
@@ -1958,7 +1957,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="2">
         <v>36002001007</v>
@@ -1986,7 +1985,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="2">
         <v>36002001006</v>
@@ -2021,7 +2020,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2">
         <v>6002032003</v>
@@ -2045,7 +2044,7 @@
     </row>
     <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="2">
         <v>36002001006</v>
@@ -2067,7 +2066,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="2">
         <v>11000001001</v>
@@ -2080,7 +2079,7 @@
     </row>
     <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="2">
         <v>39002093001</v>
@@ -2099,7 +2098,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="2">
         <v>12000053001</v>
@@ -2112,7 +2111,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2">
         <v>12000001001</v>
@@ -2130,7 +2129,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2">
         <v>35000021001</v>
@@ -2148,7 +2147,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="2">
         <v>10000027001</v>
@@ -2166,7 +2165,7 @@
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="2">
         <v>41000017001</v>
@@ -2184,7 +2183,7 @@
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="2">
         <v>12000017027</v>
@@ -2204,7 +2203,7 @@
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="2">
         <v>6008022001</v>
@@ -2228,7 +2227,7 @@
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2">
         <v>15000003001</v>
@@ -2246,7 +2245,7 @@
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="2">
         <v>36003169012</v>
@@ -2264,7 +2263,7 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="2">
         <v>48004026002</v>
@@ -2282,7 +2281,7 @@
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" s="2">
         <v>39000084001</v>
@@ -2300,7 +2299,7 @@
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2">
         <v>55003100001</v>
@@ -2318,7 +2317,7 @@
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="2">
         <v>42000094002</v>
@@ -2336,7 +2335,7 @@
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="2">
         <v>6009031001</v>
@@ -2354,7 +2353,7 @@
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="2">
         <v>13000012004</v>
@@ -2372,7 +2371,7 @@
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" s="2">
         <v>4001318001</v>
@@ -2390,7 +2389,7 @@
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" s="2">
         <v>6005009001</v>
@@ -2416,10 +2415,10 @@
     </row>
     <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2434,10 +2433,10 @@
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2452,10 +2451,10 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>

</xml_diff>

<commit_message>
Updated AEP rates to include gen charges
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B4B1B9-0FDF-4C4C-9E55-778BE294A9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E328CD80-2ED7-9C4E-B00A-2664A486EBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,9 +107,6 @@
     <t>B7, G8 - Time of Use (&lt; 10 kV)</t>
   </si>
   <si>
-    <t>Schedule GS-3 (General Service - Medium Load Factor) @ Primary Voltage</t>
-  </si>
-  <si>
     <t>Schedule LPS - Primary Voltage</t>
   </si>
   <si>
@@ -342,6 +339,9 @@
   </si>
   <si>
     <t>Rate TOU-8 at 2-50 kV - Option E</t>
+  </si>
+  <si>
+    <t>Schedule GS (Demand Metered Primary)</t>
   </si>
 </sst>
 </file>
@@ -732,8 +732,8 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -749,46 +749,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -831,7 +831,7 @@
     </row>
     <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="2">
         <v>6005025001</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="2">
         <v>6005025001</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="2">
         <v>6004010004</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="2">
         <v>32000200820</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="2">
         <v>53000776002</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="2">
         <v>12000001001</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="2">
         <v>51000161001</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="B32" s="2">
         <v>39001792001</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="2">
         <v>29001011001</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="2">
         <v>55003100001</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="2">
         <v>21000025001</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" s="2">
         <v>42005016001</v>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" s="2">
         <v>6005009001</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="2">
         <v>6009031001</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="2">
         <v>31001825002</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="2">
         <v>36007136001</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="41" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B41" s="2">
         <v>9000641001</v>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B42" s="2">
         <v>9000641001</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B43" s="2">
         <v>48003033002</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B44" s="2">
         <v>48003033002</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="2">
         <v>47000940001</v>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46" s="2">
         <v>29001023001</v>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="47" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="2">
         <v>26000596001</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="48" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B48" s="2">
         <v>39002093001</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="49" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="2">
         <v>10000027001</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="50" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50" s="2">
         <v>10000027001</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="51" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51" s="2">
         <v>10000027001</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="52" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="2">
         <v>6009031001</v>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53">
         <v>39000084001</v>
@@ -1814,25 +1814,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2">
         <v>29001023001</v>
@@ -1852,7 +1852,7 @@
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2">
         <v>36007136001</v>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2">
         <v>8000070001</v>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2">
         <v>53001280001</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2">
         <v>11000001001</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="2">
         <v>25000128001</v>
@@ -1914,7 +1914,7 @@
     </row>
     <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2">
         <v>39002093001</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="2">
         <v>39001792001</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2">
         <v>47001016001</v>
@@ -1957,7 +1957,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2">
         <v>36002001007</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="2">
         <v>36002001006</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="2">
         <v>6002032003</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="2">
         <v>36002001006</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2">
         <v>11000001001</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="2">
         <v>39002093001</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2">
         <v>12000053001</v>
@@ -2111,7 +2111,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="2">
         <v>12000001001</v>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="2">
         <v>35000021001</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="2">
         <v>10000027001</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="2">
         <v>41000017001</v>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="2">
         <v>12000017027</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="2">
         <v>6008022001</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="2">
         <v>15000003001</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="2">
         <v>36003169012</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="2">
         <v>48004026002</v>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2">
         <v>39000084001</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="2">
         <v>55003100001</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2">
         <v>42000094002</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="2">
         <v>6009031001</v>
@@ -2353,7 +2353,7 @@
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="2">
         <v>13000012004</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2">
         <v>4001318001</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="2">
         <v>6005009001</v>
@@ -2415,10 +2415,10 @@
     </row>
     <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2433,10 +2433,10 @@
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2451,10 +2451,10 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>

</xml_diff>

<commit_message>
Added Schedule EECC to SDG&E
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fletc\Git\wwtp-energy-tariffs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E328CD80-2ED7-9C4E-B00A-2664A486EBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A4281B-8D46-4330-9242-4F4A6F3DC7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electric" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
   <si>
     <t>Assumption</t>
   </si>
@@ -342,13 +342,16 @@
   </si>
   <si>
     <t>Schedule GS (Demand Metered Primary)</t>
+  </si>
+  <si>
+    <t>Schedule EECC for generation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -383,6 +386,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F2328"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -404,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -413,6 +423,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,21 +741,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1"/>
-    <col min="2" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+    <col min="2" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +802,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -799,7 +810,7 @@
         <v>12000053001</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -807,7 +818,7 @@
         <v>48003033002</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -815,7 +826,7 @@
         <v>31001825002</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -829,7 +840,7 @@
         <v>36001010006</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
@@ -852,7 +863,7 @@
         <v>6002121001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
@@ -875,7 +886,7 @@
         <v>6002121001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -894,7 +905,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>101</v>
       </c>
@@ -917,7 +928,7 @@
         <v>6004009001</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -958,7 +969,7 @@
         <v>36002001011</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -977,7 +988,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>83</v>
       </c>
@@ -998,7 +1009,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1021,7 +1032,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>84</v>
       </c>
@@ -1040,7 +1051,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1059,7 +1070,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1086,7 +1097,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>99</v>
       </c>
@@ -1111,7 +1122,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -1132,7 +1143,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -1151,7 +1162,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1170,7 +1181,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
@@ -1189,7 +1200,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
@@ -1208,7 +1219,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
@@ -1229,7 +1240,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
@@ -1252,7 +1263,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
@@ -1277,7 +1288,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>19</v>
       </c>
@@ -1296,7 +1307,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>20</v>
       </c>
@@ -1315,7 +1326,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
@@ -1334,7 +1345,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>22</v>
       </c>
@@ -1353,7 +1364,7 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
@@ -1372,7 +1383,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>82</v>
       </c>
@@ -1393,7 +1404,7 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>102</v>
       </c>
@@ -1414,7 +1425,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>24</v>
       </c>
@@ -1433,7 +1444,7 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>25</v>
       </c>
@@ -1452,7 +1463,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>26</v>
       </c>
@@ -1471,7 +1482,7 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>27</v>
       </c>
@@ -1490,7 +1501,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>28</v>
       </c>
@@ -1509,7 +1520,7 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>29</v>
       </c>
@@ -1528,7 +1539,7 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>30</v>
       </c>
@@ -1536,7 +1547,7 @@
         <v>31001825002</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1559,7 +1570,7 @@
         <v>17000721001</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>32</v>
       </c>
@@ -1570,7 +1581,7 @@
         <v>42006056001</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -1617,7 +1628,7 @@
         <v>6009031001</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>34</v>
       </c>
@@ -1658,7 +1669,7 @@
         <v>26004005011</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>35</v>
       </c>
@@ -1684,7 +1695,7 @@
         <v>34002065001</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>36</v>
       </c>
@@ -1710,7 +1721,7 @@
         <v>47001016001</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>37</v>
       </c>
@@ -1724,7 +1735,7 @@
         <v>42006056001</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>38</v>
       </c>
@@ -1735,7 +1746,7 @@
         <v>26004005011</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>39</v>
       </c>
@@ -1743,7 +1754,7 @@
         <v>39002093001</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>40</v>
       </c>
@@ -1751,7 +1762,7 @@
         <v>10000027001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>41</v>
       </c>
@@ -1762,7 +1773,7 @@
         <v>13000012004</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>42</v>
       </c>
@@ -1773,7 +1784,7 @@
         <v>29001011001</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>43</v>
       </c>
@@ -1781,7 +1792,7 @@
         <v>6009031001</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>100</v>
       </c>
@@ -1789,9 +1800,17 @@
         <v>39000084001</v>
       </c>
     </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="6">
+        <v>6009031001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToHeight="0" orientation="landscape"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1803,13 +1822,13 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.1640625" customWidth="1"/>
-    <col min="2" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" customWidth="1"/>
+    <col min="2" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1839,7 +1858,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1850,7 +1869,7 @@
         <v>29001023002</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -1864,7 +1883,7 @@
         <v>36009071001</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
@@ -1872,7 +1891,7 @@
         <v>8000070001</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>47</v>
       </c>
@@ -1886,7 +1905,7 @@
         <v>53000776002</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -1899,7 +1918,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -1912,7 +1931,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>50</v>
       </c>
@@ -1925,7 +1944,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>51</v>
       </c>
@@ -1942,7 +1961,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>52</v>
       </c>
@@ -1955,7 +1974,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1983,7 +2002,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2005,7 +2024,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>34001005001</v>
       </c>
@@ -2018,7 +2037,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -2042,7 +2061,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>56</v>
       </c>
@@ -2064,7 +2083,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>57</v>
       </c>
@@ -2077,7 +2096,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
@@ -2096,7 +2115,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -2109,7 +2128,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2127,7 +2146,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2145,7 +2164,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -2163,7 +2182,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -2181,7 +2200,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2201,7 +2220,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -2225,7 +2244,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>65</v>
       </c>
@@ -2243,7 +2262,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>66</v>
       </c>
@@ -2261,7 +2280,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>67</v>
       </c>
@@ -2279,7 +2298,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>68</v>
       </c>
@@ -2297,7 +2316,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>69</v>
       </c>
@@ -2315,7 +2334,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>70</v>
       </c>
@@ -2333,7 +2352,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>71</v>
       </c>
@@ -2351,7 +2370,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>72</v>
       </c>
@@ -2369,7 +2388,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>73</v>
       </c>
@@ -2387,7 +2406,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>81</v>
       </c>
@@ -2413,7 +2432,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>74</v>
       </c>
@@ -2431,7 +2450,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>76</v>
       </c>
@@ -2449,7 +2468,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -2467,7 +2486,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2481,7 +2500,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2495,7 +2514,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2509,7 +2528,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2523,7 +2542,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2537,7 +2556,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2551,7 +2570,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2565,11 +2584,11 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2578,10 +2597,10 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2589,7 +2608,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2599,7 +2618,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2608,13 +2627,13 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switched Facility 36008024001 to RG&E
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fletc\Git\wwtp-energy-tariffs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A4281B-8D46-4330-9242-4F4A6F3DC7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED39536C-2011-E941-A157-C251B7E59697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electric" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="106">
   <si>
     <t>Assumption</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>Schedule EECC for generation</t>
+  </si>
+  <si>
+    <t>Service Classification No. 3: General Service (100 kW minimum)</t>
+  </si>
+  <si>
+    <t>Non-retail RG&amp;E Supply Service (RSS)</t>
   </si>
 </sst>
 </file>
@@ -741,21 +747,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="2" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +808,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -810,7 +816,7 @@
         <v>12000053001</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -818,7 +824,7 @@
         <v>48003033002</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -826,7 +832,7 @@
         <v>31001825002</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -840,7 +846,7 @@
         <v>36001010006</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
@@ -863,7 +869,7 @@
         <v>6002121001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
@@ -886,7 +892,7 @@
         <v>6002121001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -905,7 +911,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>101</v>
       </c>
@@ -928,7 +934,7 @@
         <v>6004009001</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -969,7 +975,7 @@
         <v>36002001011</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -988,7 +994,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>83</v>
       </c>
@@ -1009,7 +1015,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1032,7 +1038,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>84</v>
       </c>
@@ -1051,7 +1057,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1070,7 +1076,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1097,7 +1103,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>99</v>
       </c>
@@ -1122,7 +1128,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -1143,7 +1149,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -1162,7 +1168,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1181,7 +1187,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
@@ -1200,7 +1206,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
@@ -1219,7 +1225,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
@@ -1240,7 +1246,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
@@ -1263,7 +1269,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
@@ -1288,7 +1294,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>19</v>
       </c>
@@ -1307,7 +1313,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>20</v>
       </c>
@@ -1326,7 +1332,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
@@ -1345,7 +1351,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>22</v>
       </c>
@@ -1364,7 +1370,7 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
@@ -1383,7 +1389,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>82</v>
       </c>
@@ -1404,7 +1410,7 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>102</v>
       </c>
@@ -1425,7 +1431,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>24</v>
       </c>
@@ -1444,7 +1450,7 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>25</v>
       </c>
@@ -1463,7 +1469,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>26</v>
       </c>
@@ -1482,7 +1488,7 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>27</v>
       </c>
@@ -1501,7 +1507,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>28</v>
       </c>
@@ -1520,7 +1526,7 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>29</v>
       </c>
@@ -1539,7 +1545,7 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>30</v>
       </c>
@@ -1547,7 +1553,7 @@
         <v>31001825002</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1570,7 +1576,7 @@
         <v>17000721001</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>32</v>
       </c>
@@ -1581,7 +1587,7 @@
         <v>42006056001</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -1628,7 +1634,7 @@
         <v>6009031001</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>34</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>26004005011</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>35</v>
       </c>
@@ -1695,7 +1701,7 @@
         <v>34002065001</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>36</v>
       </c>
@@ -1721,7 +1727,7 @@
         <v>47001016001</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>37</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>42006056001</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>38</v>
       </c>
@@ -1746,7 +1752,7 @@
         <v>26004005011</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>39</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>39002093001</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>40</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>10000027001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>41</v>
       </c>
@@ -1773,7 +1779,7 @@
         <v>13000012004</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>42</v>
       </c>
@@ -1784,7 +1790,7 @@
         <v>29001011001</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>43</v>
       </c>
@@ -1792,7 +1798,7 @@
         <v>6009031001</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>100</v>
       </c>
@@ -1800,12 +1806,28 @@
         <v>39000084001</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B54" s="6">
         <v>6009031001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55">
+        <v>36008024001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56">
+        <v>36008024001</v>
       </c>
     </row>
   </sheetData>
@@ -1822,13 +1844,13 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.140625" customWidth="1"/>
-    <col min="2" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.1640625" customWidth="1"/>
+    <col min="2" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1858,7 +1880,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1869,7 +1891,7 @@
         <v>29001023002</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -1883,7 +1905,7 @@
         <v>36009071001</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
@@ -1891,7 +1913,7 @@
         <v>8000070001</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>47</v>
       </c>
@@ -1905,7 +1927,7 @@
         <v>53000776002</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -1918,7 +1940,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
@@ -1931,7 +1953,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>50</v>
       </c>
@@ -1944,7 +1966,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>51</v>
       </c>
@@ -1961,7 +1983,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>52</v>
       </c>
@@ -1974,7 +1996,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -2002,7 +2024,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2024,7 +2046,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>34001005001</v>
       </c>
@@ -2037,7 +2059,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -2061,7 +2083,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>56</v>
       </c>
@@ -2083,7 +2105,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>57</v>
       </c>
@@ -2096,7 +2118,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
@@ -2115,7 +2137,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -2128,7 +2150,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2146,7 +2168,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2164,7 +2186,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -2182,7 +2204,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -2200,7 +2222,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2220,7 +2242,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -2244,7 +2266,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>65</v>
       </c>
@@ -2262,7 +2284,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>66</v>
       </c>
@@ -2280,7 +2302,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>67</v>
       </c>
@@ -2298,7 +2320,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>68</v>
       </c>
@@ -2316,7 +2338,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>69</v>
       </c>
@@ -2334,7 +2356,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>70</v>
       </c>
@@ -2352,7 +2374,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>71</v>
       </c>
@@ -2370,7 +2392,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>72</v>
       </c>
@@ -2388,7 +2410,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>73</v>
       </c>
@@ -2406,7 +2428,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>81</v>
       </c>
@@ -2432,7 +2454,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>74</v>
       </c>
@@ -2450,7 +2472,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>76</v>
       </c>
@@ -2468,7 +2490,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -2486,7 +2508,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2500,7 +2522,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2514,7 +2536,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2528,7 +2550,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2542,7 +2564,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2556,7 +2578,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2570,7 +2592,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2584,11 +2606,11 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2597,10 +2619,10 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2608,7 +2630,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2618,7 +2640,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2627,13 +2649,13 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added fuel costs to CPS energy
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED39536C-2011-E941-A157-C251B7E59697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E273B76C-CF52-0F46-949E-8B5133A75C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electric" sheetId="1" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>Regulatory, Delivery, or other charges in addition to Demand</t>
   </si>
   <si>
-    <t>Power supply charges in addtion to Energy</t>
-  </si>
-  <si>
     <t>Charge limit ignored since it was a complex equation</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>Non-retail RG&amp;E Supply Service (RSS)</t>
+  </si>
+  <si>
+    <t>Ignored fuel adjustment clause as &lt; $0.0005 / kWh</t>
   </si>
 </sst>
 </file>
@@ -749,8 +749,8 @@
   </sheetPr>
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -766,46 +766,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -848,7 +848,7 @@
     </row>
     <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="2">
         <v>6005025001</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="2">
         <v>6005025001</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="2">
         <v>6004010004</v>
@@ -996,7 +996,7 @@
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="2">
         <v>32000200820</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="2">
         <v>53000776002</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="2">
         <v>12000001001</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="2">
         <v>51000161001</v>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" s="2">
         <v>39001792001</v>
@@ -1677,33 +1677,21 @@
     </row>
     <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="B44" s="2">
-        <v>48003033002</v>
-      </c>
-      <c r="C44" s="2">
-        <v>12000001001</v>
-      </c>
-      <c r="D44" s="2">
-        <v>12000017028</v>
-      </c>
-      <c r="E44" s="2">
-        <v>12000017027</v>
-      </c>
-      <c r="F44" s="2">
-        <v>12000017004</v>
-      </c>
-      <c r="G44" s="2">
-        <v>41000017001</v>
-      </c>
-      <c r="H44" s="2">
-        <v>34002065001</v>
-      </c>
+        <v>29001011001</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B45" s="2">
         <v>47000940001</v>
@@ -1729,7 +1717,7 @@
     </row>
     <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" s="2">
         <v>29001023001</v>
@@ -1743,7 +1731,7 @@
     </row>
     <row r="47" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B47" s="2">
         <v>26000596001</v>
@@ -1754,7 +1742,7 @@
     </row>
     <row r="48" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="2">
         <v>39002093001</v>
@@ -1762,7 +1750,7 @@
     </row>
     <row r="49" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B49" s="2">
         <v>10000027001</v>
@@ -1770,7 +1758,7 @@
     </row>
     <row r="50" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="2">
         <v>10000027001</v>
@@ -1781,7 +1769,7 @@
     </row>
     <row r="51" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B51" s="2">
         <v>10000027001</v>
@@ -1792,7 +1780,7 @@
     </row>
     <row r="52" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B52" s="2">
         <v>6009031001</v>
@@ -1800,7 +1788,7 @@
     </row>
     <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B53">
         <v>39000084001</v>
@@ -1808,7 +1796,7 @@
     </row>
     <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="6">
         <v>6009031001</v>
@@ -1816,7 +1804,7 @@
     </row>
     <row r="55" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55">
         <v>36008024001</v>
@@ -1824,7 +1812,7 @@
     </row>
     <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56">
         <v>36008024001</v>
@@ -1840,7 +1828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85995C10-2ADA-4E06-99AB-80C6038BFB63}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1855,25 +1843,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1882,7 +1870,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2">
         <v>29001023001</v>
@@ -1893,7 +1881,7 @@
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2">
         <v>36007136001</v>
@@ -1907,7 +1895,7 @@
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2">
         <v>8000070001</v>
@@ -1915,7 +1903,7 @@
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2">
         <v>53001280001</v>
@@ -1929,7 +1917,7 @@
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2">
         <v>11000001001</v>
@@ -1942,7 +1930,7 @@
     </row>
     <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2">
         <v>25000128001</v>
@@ -1955,7 +1943,7 @@
     </row>
     <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2">
         <v>39002093001</v>
@@ -1968,7 +1956,7 @@
     </row>
     <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2">
         <v>39001792001</v>
@@ -1985,7 +1973,7 @@
     </row>
     <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2">
         <v>47001016001</v>
@@ -1998,7 +1986,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2">
         <v>36002001007</v>
@@ -2026,7 +2014,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2">
         <v>36002001006</v>
@@ -2061,7 +2049,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="2">
         <v>6002032003</v>
@@ -2085,7 +2073,7 @@
     </row>
     <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="2">
         <v>36002001006</v>
@@ -2107,7 +2095,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="2">
         <v>11000001001</v>
@@ -2120,7 +2108,7 @@
     </row>
     <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2">
         <v>39002093001</v>
@@ -2139,7 +2127,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="2">
         <v>12000053001</v>
@@ -2152,7 +2140,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2">
         <v>12000001001</v>
@@ -2170,7 +2158,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="2">
         <v>35000021001</v>
@@ -2188,7 +2176,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2">
         <v>10000027001</v>
@@ -2206,7 +2194,7 @@
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="2">
         <v>41000017001</v>
@@ -2224,7 +2212,7 @@
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="2">
         <v>12000017027</v>
@@ -2244,7 +2232,7 @@
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="2">
         <v>6008022001</v>
@@ -2268,7 +2256,7 @@
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="2">
         <v>15000003001</v>
@@ -2286,7 +2274,7 @@
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="2">
         <v>36003169012</v>
@@ -2304,7 +2292,7 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="2">
         <v>48004026002</v>
@@ -2322,7 +2310,7 @@
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2">
         <v>39000084001</v>
@@ -2340,7 +2328,7 @@
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="2">
         <v>55003100001</v>
@@ -2358,7 +2346,7 @@
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="2">
         <v>42000094002</v>
@@ -2376,7 +2364,7 @@
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2">
         <v>6009031001</v>
@@ -2394,7 +2382,7 @@
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="2">
         <v>13000012004</v>
@@ -2412,7 +2400,7 @@
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="2">
         <v>4001318001</v>
@@ -2430,7 +2418,7 @@
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" s="2">
         <v>6005009001</v>
@@ -2456,10 +2444,10 @@
     </row>
     <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2474,10 +2462,10 @@
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2492,10 +2480,10 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>

</xml_diff>

<commit_message>
Finished updating assumptions spreadsheet
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E273B76C-CF52-0F46-949E-8B5133A75C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561E4410-122D-E94F-88B5-D510F58DD5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electric" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
   <si>
     <t>Assumption</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Standard Voltage (b/c primary had a minimum demand of 10 MW)</t>
   </si>
   <si>
-    <t>Live time-of-use pricing</t>
-  </si>
-  <si>
     <t>Ignored peak hours shift with daylight savings</t>
   </si>
   <si>
@@ -351,6 +348,27 @@
   </si>
   <si>
     <t>Ignored fuel adjustment clause as &lt; $0.0005 / kWh</t>
+  </si>
+  <si>
+    <t>Chose 12-month fixed-rate delivery service contract from open market due to ERCOT deregulation rules</t>
+  </si>
+  <si>
+    <t>CWNS_No_15</t>
+  </si>
+  <si>
+    <t>CWNS_No_16</t>
+  </si>
+  <si>
+    <t>CWNS_No_17</t>
+  </si>
+  <si>
+    <t>CWNS_No_18</t>
+  </si>
+  <si>
+    <t>Live time-of-use pricing, so averaged NYISO locational marginal price with same granularity as underlying TOU rate structure</t>
+  </si>
+  <si>
+    <t>Live time-of-use pricing, so averaged PJM locational-marginal price with same granularity as underlying TOU rate structure</t>
   </si>
 </sst>
 </file>
@@ -747,10 +765,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -759,56 +777,69 @@
     <col min="2" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -816,7 +847,7 @@
         <v>12000053001</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -824,7 +855,7 @@
         <v>48003033002</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -832,7 +863,7 @@
         <v>31001825002</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -846,9 +877,9 @@
         <v>36001010006</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="2">
         <v>6005025001</v>
@@ -869,9 +900,9 @@
         <v>6002121001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2">
         <v>6005025001</v>
@@ -892,7 +923,7 @@
         <v>6002121001</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -911,9 +942,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" s="2">
         <v>6004010004</v>
@@ -934,7 +965,7 @@
         <v>6004009001</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -975,7 +1006,7 @@
         <v>36002001011</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -994,9 +1025,9 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="2">
         <v>32000200820</v>
@@ -1015,7 +1046,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1038,9 +1069,9 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" s="2">
         <v>53000776002</v>
@@ -1057,7 +1088,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1076,7 +1107,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1105,7 +1136,7 @@
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="2">
         <v>12000001001</v>
@@ -1391,7 +1422,7 @@
     </row>
     <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="2">
         <v>51000161001</v>
@@ -1412,7 +1443,7 @@
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="2">
         <v>39001792001</v>
@@ -1431,7 +1462,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>24</v>
       </c>
@@ -1450,7 +1481,7 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>25</v>
       </c>
@@ -1469,7 +1500,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>26</v>
       </c>
@@ -1488,7 +1519,7 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>27</v>
       </c>
@@ -1507,7 +1538,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>28</v>
       </c>
@@ -1526,7 +1557,7 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>29</v>
       </c>
@@ -1545,7 +1576,7 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>30</v>
       </c>
@@ -1553,269 +1584,369 @@
         <v>31001825002</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40">
+        <v>42006056001</v>
+      </c>
+      <c r="C40">
+        <v>42000094003</v>
+      </c>
+      <c r="D40">
+        <v>42000094002</v>
+      </c>
+      <c r="E40">
+        <v>42000094001</v>
+      </c>
+      <c r="F40">
+        <v>42005016001</v>
+      </c>
+      <c r="G40" s="2">
+        <v>17000721009</v>
+      </c>
+      <c r="H40" s="2">
+        <v>17000721007</v>
+      </c>
+      <c r="I40" s="2">
+        <v>17000721001</v>
+      </c>
+      <c r="J40">
+        <v>34001082001</v>
+      </c>
+      <c r="K40">
+        <v>34002065001</v>
+      </c>
+      <c r="L40">
+        <v>34006012001</v>
+      </c>
+      <c r="M40">
+        <v>34001005001</v>
+      </c>
+      <c r="N40">
+        <v>34001030001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="2">
+        <v>36007136001</v>
+      </c>
+      <c r="C41" s="2">
+        <v>36008024001</v>
+      </c>
+      <c r="D41" s="2">
+        <v>36009071001</v>
+      </c>
+      <c r="E41" s="2">
+        <v>36002001007</v>
+      </c>
+      <c r="F41" s="2">
+        <v>36002001004</v>
+      </c>
+      <c r="G41" s="2">
+        <v>36002001006</v>
+      </c>
+      <c r="H41" s="2">
+        <v>36003169012</v>
+      </c>
+      <c r="I41" s="2">
+        <v>36002001010</v>
+      </c>
+      <c r="J41" s="2">
+        <v>36002001009</v>
+      </c>
+      <c r="K41" s="2">
+        <v>36002001005</v>
+      </c>
+      <c r="L41" s="2">
+        <v>36002001002</v>
+      </c>
+      <c r="M41" s="2">
+        <v>36002001003</v>
+      </c>
+      <c r="N41" s="2">
+        <v>36002001012</v>
+      </c>
+      <c r="O41" s="2">
+        <v>36002001001</v>
+      </c>
+      <c r="P41" s="2">
+        <v>36002001011</v>
+      </c>
+      <c r="Q41">
+        <v>36001010001</v>
+      </c>
+      <c r="R41">
+        <v>36001010017</v>
+      </c>
+      <c r="S41">
+        <v>36001010006</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B40" s="2">
-        <v>36007136001</v>
-      </c>
-      <c r="C40" s="2">
-        <v>36008024001</v>
-      </c>
-      <c r="D40" s="2">
-        <v>36009071001</v>
-      </c>
-      <c r="E40" s="2">
-        <v>17000721009</v>
-      </c>
-      <c r="F40" s="2">
-        <v>17000721007</v>
-      </c>
-      <c r="G40" s="2">
-        <v>17000721001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" s="2">
-        <v>9000641001</v>
-      </c>
-      <c r="C41" s="2">
-        <v>42006056001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>33</v>
       </c>
       <c r="B42" s="2">
         <v>9000641001</v>
       </c>
       <c r="C42" s="2">
+        <v>42006056001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="2">
+        <v>9000641001</v>
+      </c>
+      <c r="C43" s="2">
         <v>51000161001</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D43" s="2">
         <v>51000154002</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E43" s="2">
         <v>39001666001</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F43" s="2">
         <v>39001666002</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G43" s="2">
         <v>39000084001</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H43" s="2">
         <v>39008260001</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I43" s="2">
         <v>39001792001</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J43" s="2">
         <v>39001792002</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K43" s="2">
         <v>29001023001</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L43" s="2">
         <v>29001023002</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M43" s="2">
         <v>53000776001</v>
       </c>
-      <c r="N42" s="2">
+      <c r="N43" s="2">
         <v>47001016001</v>
       </c>
-      <c r="O42" s="2">
+      <c r="O43" s="2">
         <v>6009031001</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+    <row r="44" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="2">
+        <v>48003033002</v>
+      </c>
+      <c r="C44" s="2">
+        <v>9000641001</v>
+      </c>
+      <c r="D44" s="2">
+        <v>12000001001</v>
+      </c>
+      <c r="E44" s="2">
+        <v>12000017028</v>
+      </c>
+      <c r="F44" s="2">
+        <v>12000017027</v>
+      </c>
+      <c r="G44" s="2">
+        <v>12000017004</v>
+      </c>
+      <c r="H44" s="2">
+        <v>32000011001</v>
+      </c>
+      <c r="I44" s="2">
+        <v>32000200820</v>
+      </c>
+      <c r="J44" s="2">
+        <v>41000017001</v>
+      </c>
+      <c r="K44" s="2">
+        <v>24000001002</v>
+      </c>
+      <c r="L44" s="2">
+        <v>26000596001</v>
+      </c>
+      <c r="M44" s="2">
+        <v>26004005011</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="2">
+        <v>29001011001</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="2">
-        <v>48003033002</v>
-      </c>
-      <c r="C43" s="2">
-        <v>9000641001</v>
-      </c>
-      <c r="D43" s="2">
-        <v>12000001001</v>
-      </c>
-      <c r="E43" s="2">
-        <v>12000017028</v>
-      </c>
-      <c r="F43" s="2">
-        <v>12000017027</v>
-      </c>
-      <c r="G43" s="2">
-        <v>12000017004</v>
-      </c>
-      <c r="H43" s="2">
-        <v>32000011001</v>
-      </c>
-      <c r="I43" s="2">
-        <v>32000200820</v>
-      </c>
-      <c r="J43" s="2">
-        <v>41000017001</v>
-      </c>
-      <c r="K43" s="2">
-        <v>24000001002</v>
-      </c>
-      <c r="L43" s="2">
+      <c r="B46" s="2">
+        <v>47000940001</v>
+      </c>
+      <c r="C46" s="2">
+        <v>47000940002</v>
+      </c>
+      <c r="D46" s="2">
+        <v>47000245002</v>
+      </c>
+      <c r="E46" s="2">
         <v>26000596001</v>
       </c>
-      <c r="M43" s="2">
+      <c r="F46" s="2">
         <v>26004005011</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B44" s="2">
+      <c r="G46" s="2">
         <v>29001011001</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-    </row>
-    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="H46" s="2">
+        <v>47001016001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="2">
-        <v>47000940001</v>
-      </c>
-      <c r="C45" s="2">
-        <v>47000940002</v>
-      </c>
-      <c r="D45" s="2">
-        <v>47000245002</v>
-      </c>
-      <c r="E45" s="2">
+      <c r="B47" s="2">
+        <v>29001023001</v>
+      </c>
+      <c r="C47" s="2">
+        <v>29001023002</v>
+      </c>
+      <c r="D47" s="2">
+        <v>42006056001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="2">
         <v>26000596001</v>
       </c>
-      <c r="F45" s="2">
+      <c r="C48" s="2">
         <v>26004005011</v>
       </c>
-      <c r="G45" s="2">
-        <v>29001011001</v>
-      </c>
-      <c r="H45" s="2">
-        <v>47001016001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B46" s="2">
-        <v>29001023001</v>
-      </c>
-      <c r="C46" s="2">
-        <v>29001023002</v>
-      </c>
-      <c r="D46" s="2">
-        <v>42006056001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+    </row>
+    <row r="49" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="2">
-        <v>26000596001</v>
-      </c>
-      <c r="C47" s="2">
-        <v>26004005011</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+      <c r="B49" s="2">
+        <v>39002093001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B48" s="2">
-        <v>39002093001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" s="2">
-        <v>10000027001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="B50" s="2">
         <v>10000027001</v>
       </c>
-      <c r="C50" s="2">
-        <v>13000012004</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B51" s="2">
         <v>10000027001</v>
       </c>
       <c r="C51" s="2">
+        <v>13000012004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="2">
+        <v>10000027001</v>
+      </c>
+      <c r="C52" s="2">
         <v>29001011001</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="2">
+    <row r="53" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="2">
         <v>6009031001</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B53">
+    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54">
         <v>39000084001</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="6">
+        <v>6009031001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="B54" s="6">
-        <v>6009031001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B55">
-        <v>36008024001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="B56">
         <v>36008024001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57">
+        <v>36008024001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58">
+        <v>48004026002</v>
+      </c>
+      <c r="C58">
+        <v>48007039001</v>
+      </c>
+      <c r="D58">
+        <v>48004026001</v>
+      </c>
+      <c r="E58">
+        <v>48004122001</v>
+      </c>
+      <c r="F58">
+        <v>48000004001</v>
       </c>
     </row>
   </sheetData>
@@ -1843,25 +1974,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1870,7 +2001,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2">
         <v>29001023001</v>
@@ -1881,7 +2012,7 @@
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2">
         <v>36007136001</v>
@@ -1895,7 +2026,7 @@
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2">
         <v>8000070001</v>
@@ -1903,7 +2034,7 @@
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2">
         <v>53001280001</v>
@@ -1917,7 +2048,7 @@
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="2">
         <v>11000001001</v>
@@ -1930,7 +2061,7 @@
     </row>
     <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="2">
         <v>25000128001</v>
@@ -1943,7 +2074,7 @@
     </row>
     <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="2">
         <v>39002093001</v>
@@ -1956,7 +2087,7 @@
     </row>
     <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2">
         <v>39001792001</v>
@@ -1973,7 +2104,7 @@
     </row>
     <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="2">
         <v>47001016001</v>
@@ -1986,7 +2117,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2">
         <v>36002001007</v>
@@ -2014,7 +2145,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="2">
         <v>36002001006</v>
@@ -2049,7 +2180,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="2">
         <v>6002032003</v>
@@ -2073,7 +2204,7 @@
     </row>
     <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="2">
         <v>36002001006</v>
@@ -2095,7 +2226,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2">
         <v>11000001001</v>
@@ -2108,7 +2239,7 @@
     </row>
     <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="2">
         <v>39002093001</v>
@@ -2127,7 +2258,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" s="2">
         <v>12000053001</v>
@@ -2140,7 +2271,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2">
         <v>12000001001</v>
@@ -2158,7 +2289,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="2">
         <v>35000021001</v>
@@ -2176,7 +2307,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="2">
         <v>10000027001</v>
@@ -2194,7 +2325,7 @@
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="2">
         <v>41000017001</v>
@@ -2212,7 +2343,7 @@
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="2">
         <v>12000017027</v>
@@ -2232,7 +2363,7 @@
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="2">
         <v>6008022001</v>
@@ -2256,7 +2387,7 @@
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="2">
         <v>15000003001</v>
@@ -2274,7 +2405,7 @@
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="2">
         <v>36003169012</v>
@@ -2292,7 +2423,7 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="2">
         <v>48004026002</v>
@@ -2310,7 +2441,7 @@
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" s="2">
         <v>39000084001</v>
@@ -2328,7 +2459,7 @@
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="2">
         <v>55003100001</v>
@@ -2346,7 +2477,7 @@
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="2">
         <v>42000094002</v>
@@ -2364,7 +2495,7 @@
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="2">
         <v>6009031001</v>
@@ -2382,7 +2513,7 @@
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2">
         <v>13000012004</v>
@@ -2400,7 +2531,7 @@
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="2">
         <v>4001318001</v>
@@ -2418,7 +2549,7 @@
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="2">
         <v>6005009001</v>
@@ -2444,10 +2575,10 @@
     </row>
     <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2462,10 +2593,10 @@
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2480,10 +2611,10 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>

</xml_diff>

<commit_message>
Added TVA assumption to list
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561E4410-122D-E94F-88B5-D510F58DD5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA446EA-AC32-CF4E-816C-E932ADFDA5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electric" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="113">
   <si>
     <t>Assumption</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>Live time-of-use pricing, so averaged PJM locational-marginal price with same granularity as underlying TOU rate structure</t>
+  </si>
+  <si>
+    <t>TVA fuel cost adjustment</t>
   </si>
 </sst>
 </file>
@@ -765,10 +768,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1947,6 +1950,23 @@
       </c>
       <c r="F58">
         <v>48000004001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59">
+        <v>47000245002</v>
+      </c>
+      <c r="C59">
+        <v>47000940001</v>
+      </c>
+      <c r="D59">
+        <v>47000940002</v>
+      </c>
+      <c r="E59">
+        <v>47001016001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final changes to references
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA446EA-AC32-CF4E-816C-E932ADFDA5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF9CC6C-BBFD-FF4C-A029-4ED41A1AD30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="114">
   <si>
     <t>Assumption</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>TVA fuel cost adjustment</t>
+  </si>
+  <si>
+    <t>Total Monthly Fuel Cost Adjusment (TMFCA)</t>
   </si>
 </sst>
 </file>
@@ -768,10 +771,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S59"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1957,16 +1960,21 @@
         <v>112</v>
       </c>
       <c r="B59">
+        <v>47000940001</v>
+      </c>
+      <c r="C59">
+        <v>47000940002</v>
+      </c>
+      <c r="D59">
+        <v>47001016001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60">
         <v>47000245002</v>
-      </c>
-      <c r="C59">
-        <v>47000940001</v>
-      </c>
-      <c r="D59">
-        <v>47000940002</v>
-      </c>
-      <c r="E59">
-        <v>47001016001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated metadata and assumptions with new suppliers
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing_Assumptions.xlsx
+++ b/data/WWTP_Billing_Assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF9CC6C-BBFD-FF4C-A029-4ED41A1AD30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C56B2DF-22CE-C44D-9E47-EFF1B78143D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electric" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="130">
   <si>
     <t>Assumption</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Large Volume Service (Cogeneration)</t>
   </si>
   <si>
-    <t>Large General (SC-3)</t>
-  </si>
-  <si>
     <t>Large Commercial (CLG)</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t xml:space="preserve">CHP uses 90% biogas, 10% natural gas </t>
   </si>
   <si>
-    <t>Ignore gas if no CHP</t>
-  </si>
-  <si>
     <t>Industrial Rate B-20 at Primary Voltage</t>
   </si>
   <si>
@@ -272,9 +266,6 @@
     <t>Schedule GS-3</t>
   </si>
   <si>
-    <t>G-NR2</t>
-  </si>
-  <si>
     <t>Schedule GS-4: Large General Service @ Primary Voltage</t>
   </si>
   <si>
@@ -375,13 +366,70 @@
   </si>
   <si>
     <t>Total Monthly Fuel Cost Adjusment (TMFCA)</t>
+  </si>
+  <si>
+    <t>Commercial Service Rate</t>
+  </si>
+  <si>
+    <t>Schedule B - Commercial &amp; Industrial Firm Service</t>
+  </si>
+  <si>
+    <t>SC 15</t>
+  </si>
+  <si>
+    <t>Rate LGS (Commercial/Industrial Large General Service)</t>
+  </si>
+  <si>
+    <t>SC3 Large General Service</t>
+  </si>
+  <si>
+    <t>SC 1 (Non Residential)</t>
+  </si>
+  <si>
+    <t>Rate Schedule LVG: Large Volume Service</t>
+  </si>
+  <si>
+    <t>Schedule 2B - General Firm Gas Sales Service</t>
+  </si>
+  <si>
+    <t>200-LCI (Large Sales - 150 Dth but less than 5,000 Dth annually)</t>
+  </si>
+  <si>
+    <t>General Gas Service - 3</t>
+  </si>
+  <si>
+    <t>C-2: Medium Commercial and Industrial General Service</t>
+  </si>
+  <si>
+    <t>Large Commercial/Public Authority &gt; 1,000 Mcf/Year</t>
+  </si>
+  <si>
+    <t>Schedules G8 &amp; G9: Large General Service</t>
+  </si>
+  <si>
+    <t>Rate GS-2</t>
+  </si>
+  <si>
+    <t>Large Volume Service</t>
+  </si>
+  <si>
+    <t>Gas Rate No. D5 - Large Volume Delivery Service</t>
+  </si>
+  <si>
+    <t>Large Commercial (&gt; 6,000 therms)</t>
+  </si>
+  <si>
+    <t>Rate 4 - Large Volume Demand Service</t>
+  </si>
+  <si>
+    <t>Rate LGSS - Large General Sales Service (Annual throughput &gt; 110,000 thm and &lt;= 540,000 thm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -423,6 +471,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -444,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -454,6 +508,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -791,58 +849,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -885,7 +943,7 @@
     </row>
     <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2">
         <v>6005025001</v>
@@ -908,7 +966,7 @@
     </row>
     <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2">
         <v>6005025001</v>
@@ -950,7 +1008,7 @@
     </row>
     <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B9" s="2">
         <v>6004010004</v>
@@ -1033,7 +1091,7 @@
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B12" s="2">
         <v>32000200820</v>
@@ -1077,7 +1135,7 @@
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" s="2">
         <v>53000776002</v>
@@ -1142,7 +1200,7 @@
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B17" s="2">
         <v>12000001001</v>
@@ -1428,7 +1486,7 @@
     </row>
     <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B31" s="2">
         <v>51000161001</v>
@@ -1449,7 +1507,7 @@
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B32" s="2">
         <v>39001792001</v>
@@ -1592,7 +1650,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B40">
         <v>42006056001</v>
@@ -1636,7 +1694,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B41" s="2">
         <v>36007136001</v>
@@ -1794,7 +1852,7 @@
     </row>
     <row r="45" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B45" s="2">
         <v>29001011001</v>
@@ -1905,7 +1963,7 @@
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B54">
         <v>39000084001</v>
@@ -1913,7 +1971,7 @@
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B55" s="6">
         <v>6009031001</v>
@@ -1921,7 +1979,7 @@
     </row>
     <row r="56" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B56">
         <v>36008024001</v>
@@ -1929,7 +1987,7 @@
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B57">
         <v>36008024001</v>
@@ -1937,7 +1995,7 @@
     </row>
     <row r="58" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B58">
         <v>48004026002</v>
@@ -1957,7 +2015,7 @@
     </row>
     <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B59">
         <v>47000940001</v>
@@ -1971,7 +2029,7 @@
     </row>
     <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B60">
         <v>47000245002</v>
@@ -1985,15 +2043,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85995C10-2ADA-4E06-99AB-80C6038BFB63}">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.1640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5" customWidth="1"/>
     <col min="2" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2002,25 +2060,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -2043,13 +2101,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="2">
-        <v>36007136001</v>
-      </c>
-      <c r="C3" s="2">
-        <v>36008024001</v>
-      </c>
-      <c r="D3" s="2">
-        <v>36009071001</v>
+        <v>8000070001</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2057,7 +2109,13 @@
         <v>44</v>
       </c>
       <c r="B4" s="2">
-        <v>8000070001</v>
+        <v>53001280001</v>
+      </c>
+      <c r="C4" s="2">
+        <v>53000776001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>53000776002</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2065,21 +2123,20 @@
         <v>45</v>
       </c>
       <c r="B5" s="2">
-        <v>53001280001</v>
-      </c>
-      <c r="C5" s="2">
-        <v>53000776001</v>
-      </c>
-      <c r="D5" s="2">
-        <v>53000776002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>11000001001</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="2">
-        <v>11000001001</v>
+        <v>25000128001</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -2087,12 +2144,12 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="2">
-        <v>25000128001</v>
+        <v>39002093001</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2105,78 +2162,85 @@
         <v>48</v>
       </c>
       <c r="B8" s="2">
-        <v>39002093001</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+        <v>39001792001</v>
+      </c>
+      <c r="C8" s="2">
+        <v>39008260001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>39001792002</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="2">
-        <v>39001792001</v>
-      </c>
-      <c r="C9" s="2">
-        <v>39008260001</v>
-      </c>
-      <c r="D9" s="2">
-        <v>39001792002</v>
-      </c>
+        <v>47001016001</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="2">
-        <v>47001016001</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+        <v>36002001007</v>
+      </c>
+      <c r="C10" s="2">
+        <v>36002001006</v>
+      </c>
+      <c r="D10" s="2">
+        <v>36002001010</v>
+      </c>
+      <c r="E10" s="2">
+        <v>36002001009</v>
+      </c>
+      <c r="F10" s="2">
+        <v>36002001005</v>
+      </c>
+      <c r="G10" s="2">
+        <v>36002001003</v>
+      </c>
+      <c r="H10" s="2">
+        <v>36002001011</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="2">
-        <v>36002001007</v>
+        <v>36003169012</v>
       </c>
       <c r="C11" s="2">
-        <v>36002001006</v>
+        <v>36002001002</v>
       </c>
       <c r="D11" s="2">
-        <v>36002001010</v>
+        <v>36002001012</v>
       </c>
       <c r="E11" s="2">
-        <v>36002001009</v>
-      </c>
-      <c r="F11" s="2">
-        <v>36002001005</v>
-      </c>
-      <c r="G11" s="2">
-        <v>36002001003</v>
-      </c>
-      <c r="H11" s="2">
-        <v>36002001011</v>
-      </c>
+        <v>36002001001</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>52</v>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B12" s="2">
-        <v>36002001006</v>
+        <v>36003169012</v>
       </c>
       <c r="C12" s="2">
         <v>36002001002</v>
@@ -2193,116 +2257,111 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="B13" s="2">
-        <v>34001005001</v>
+        <v>11000001001</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>53</v>
+    </row>
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B14" s="2">
-        <v>6002032003</v>
+        <v>39002093001</v>
       </c>
       <c r="C14" s="2">
-        <v>6002041001</v>
+        <v>39001792001</v>
       </c>
       <c r="D14" s="2">
-        <v>6002121001</v>
+        <v>39008260001</v>
       </c>
       <c r="E14" s="2">
-        <v>6002036001</v>
-      </c>
-      <c r="F14" s="2">
-        <v>6005053001</v>
-      </c>
+        <v>39001792002</v>
+      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>54</v>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>76</v>
       </c>
       <c r="B15" s="2">
-        <v>36002001006</v>
-      </c>
-      <c r="C15" s="2">
-        <v>36002001002</v>
-      </c>
-      <c r="D15" s="2">
-        <v>36002001012</v>
-      </c>
-      <c r="E15" s="2">
-        <v>36002001001</v>
-      </c>
+        <v>12000053001</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>55</v>
+      <c r="A16" t="s">
+        <v>56</v>
       </c>
       <c r="B16" s="2">
-        <v>11000001001</v>
+        <v>12000001001</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>56</v>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>57</v>
       </c>
       <c r="B17" s="2">
-        <v>39002093001</v>
-      </c>
-      <c r="C17" s="2">
-        <v>39001792001</v>
-      </c>
-      <c r="D17" s="2">
-        <v>39008260001</v>
-      </c>
-      <c r="E17" s="2">
-        <v>39001792002</v>
-      </c>
+        <v>35000021001</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2">
-        <v>12000053001</v>
+        <v>10000027001</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B19" s="2">
-        <v>12000001001</v>
+        <v>41000017001</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2317,12 +2376,14 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B20" s="2">
-        <v>35000021001</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>12000017027</v>
+      </c>
+      <c r="C20" s="2">
+        <v>12000017004</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2335,28 +2396,38 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B21" s="2">
-        <v>10000027001</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+        <v>6008022001</v>
+      </c>
+      <c r="C21" s="2">
+        <v>6008022002</v>
+      </c>
+      <c r="D21" s="2">
+        <v>6004010001</v>
+      </c>
+      <c r="E21" s="2">
+        <v>6004009001</v>
+      </c>
+      <c r="F21" s="2">
+        <v>6004010004</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6004009003</v>
+      </c>
+      <c r="H21" s="7"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>60</v>
+    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="B22" s="2">
-        <v>41000017001</v>
+        <v>15000003001</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2369,16 +2440,14 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>61</v>
+    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="B23" s="2">
-        <v>12000017027</v>
-      </c>
-      <c r="C23" s="2">
-        <v>12000017004</v>
-      </c>
+        <v>36003169012</v>
+      </c>
+      <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -2390,21 +2459,15 @@
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>62</v>
+      <c r="A24" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="B24" s="2">
-        <v>6008022001</v>
-      </c>
-      <c r="C24" s="2">
-        <v>6008022002</v>
-      </c>
-      <c r="D24" s="2">
-        <v>6004010001</v>
-      </c>
-      <c r="E24" s="2">
-        <v>6004009001</v>
-      </c>
+        <v>48004026002</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -2413,12 +2476,12 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B25" s="2">
-        <v>15000003001</v>
+        <v>39000084001</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2431,16 +2494,16 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B26" s="2">
-        <v>36003169012</v>
+        <v>55003100001</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -2451,10 +2514,10 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B27" s="2">
-        <v>48004026002</v>
+        <v>42000094002</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -2469,10 +2532,10 @@
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2">
-        <v>39000084001</v>
+        <v>6009031001</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -2485,16 +2548,16 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B29" s="2">
-        <v>55003100001</v>
+        <v>13000012004</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -2503,12 +2566,12 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2">
-        <v>42000094002</v>
+        <v>4001318001</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2522,18 +2585,30 @@
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>69</v>
+      <c r="A31" t="s">
+        <v>52</v>
       </c>
       <c r="B31" s="2">
-        <v>6009031001</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+        <v>6005009001</v>
+      </c>
+      <c r="C31" s="2">
+        <v>6005025001</v>
+      </c>
+      <c r="D31">
+        <v>6002032003</v>
+      </c>
+      <c r="E31" s="2">
+        <v>6002036001</v>
+      </c>
+      <c r="F31" s="2">
+        <v>6002121001</v>
+      </c>
+      <c r="G31" s="2">
+        <v>6002041001</v>
+      </c>
+      <c r="H31" s="2">
+        <v>6005053001</v>
+      </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -2541,14 +2616,13 @@
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B32" s="2">
-        <v>13000012004</v>
+        <v>48003033002</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="5"/>
+      <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2557,15 +2631,14 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="B33" s="2">
-        <v>4001318001</v>
+        <v>31001825002</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2577,23 +2650,19 @@
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="B34" s="2">
-        <v>6005009001</v>
+        <v>36001010001</v>
       </c>
       <c r="C34" s="2">
-        <v>6005025001</v>
+        <v>36001010017</v>
       </c>
       <c r="D34">
-        <v>6002032003</v>
-      </c>
-      <c r="E34" s="2">
-        <v>6002036001</v>
-      </c>
-      <c r="F34" s="2">
-        <v>6002121001</v>
-      </c>
+        <v>36001010006</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -2601,15 +2670,14 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>73</v>
+        <v>114</v>
+      </c>
+      <c r="B35" s="2">
+        <v>35000021001</v>
       </c>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2621,13 +2689,14 @@
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="B36">
+        <v>36007136001</v>
+      </c>
+      <c r="C36">
+        <v>36009071001</v>
+      </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -2637,15 +2706,14 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>73</v>
+    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37">
+        <v>36008024001</v>
       </c>
       <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2656,12 +2724,24 @@
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="A38" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="2">
+        <v>34001082001</v>
+      </c>
+      <c r="C38" s="2">
+        <v>34002065001</v>
+      </c>
+      <c r="D38">
+        <v>34001030001</v>
+      </c>
+      <c r="E38" s="2">
+        <v>34001005001</v>
+      </c>
+      <c r="F38" s="2">
+        <v>34006012001</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -2670,10 +2750,15 @@
       <c r="L38" s="2"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="A39" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="2">
+        <v>51000161001</v>
+      </c>
+      <c r="C39" s="2">
+        <v>51000154002</v>
+      </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -2683,11 +2768,14 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="2"/>
+    <row r="40" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" s="2">
+        <v>40000123012</v>
+      </c>
       <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -2697,10 +2785,16 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="2">
+        <v>32000011001</v>
+      </c>
+      <c r="C41" s="2">
+        <v>32000200820</v>
+      </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -2712,8 +2806,12 @@
       <c r="L41" s="2"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="2"/>
+      <c r="A42" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="2">
+        <v>47000245002</v>
+      </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2725,9 +2823,13 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="2"/>
+    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="2">
+        <v>42006056001</v>
+      </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2740,9 +2842,15 @@
       <c r="L43" s="2"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="A44" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44">
+        <v>47000940001</v>
+      </c>
+      <c r="C44" s="2">
+        <v>47000940002</v>
+      </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -2753,32 +2861,91 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" s="2">
+        <v>26004005011</v>
+      </c>
+      <c r="C45" s="2">
+        <v>26000596001</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="2">
+        <v>29001011001</v>
+      </c>
+      <c r="C46" s="2">
+        <v>29001023001</v>
+      </c>
+      <c r="D46" s="2">
+        <v>29001023002</v>
+      </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="2">
+        <v>18000061001</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" s="2">
+        <v>42005016001</v>
+      </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B49" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49">
+        <v>27000001001</v>
+      </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2786,24 +2953,91 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50">
+        <v>17000721009</v>
+      </c>
+      <c r="C50" s="2">
+        <v>17000721007</v>
+      </c>
+      <c r="D50" s="2">
+        <v>17000721001</v>
+      </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" s="3"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>